<commit_message>
Loop gestart, stopt na 1 volledige iteratie (col + row). Model moet buiten de loop runnen, anders pakt hij de rij constraints niet mee in de col loop
</commit_message>
<xml_diff>
--- a/NetworkScheduling/Assignment 1/2. Passengers/Input.xlsx
+++ b/NetworkScheduling/Assignment 1/2. Passengers/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\Desktop\NS - offline\Assignment 1\2. Passengers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C127B3C-FD78-4A39-95E1-3CF3F8785374}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{276486E2-BA92-42C9-81CD-3E8B2F0B664D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5028" yWindow="1044" windowWidth="17280" windowHeight="8964" tabRatio="917" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="917" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4175" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="291">
   <si>
     <t>Flight Number</t>
   </si>
@@ -906,6 +906,12 @@
   <si>
     <t>AR9999</t>
   </si>
+  <si>
+    <t>HALLO</t>
+  </si>
+  <si>
+    <t>METGERT</t>
+  </si>
 </sst>
 </file>
 
@@ -1378,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:H234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7450,6 +7456,32 @@
       </c>
       <c r="H233" s="6">
         <v>24</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>232</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E234" s="6">
+        <v>0</v>
+      </c>
+      <c r="F234" s="6">
+        <v>0</v>
+      </c>
+      <c r="G234" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H234" s="6">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -7468,7 +7500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A722" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A711" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I741" sqref="I741"/>
     </sheetView>
   </sheetViews>
@@ -33400,14 +33432,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B236" sqref="B236"/>
+    <sheetView topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>